<commit_message>
mobility-theme: v1.0.1 and add sections (#5)
</commit_message>
<xml_diff>
--- a/mobility-theme/mobility-theme.xlsx
+++ b/mobility-theme/mobility-theme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabularies\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70D88FE-C550-46E7-A4E9-E5ED3C848317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B15C8CE-EA0E-48B6-B08D-84EED5D6722B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>https://creativecommons.org/licenses/by/4.0/</t>
   </si>
   <si>
-    <t>My comments (not parsed by the tool).</t>
-  </si>
-  <si>
     <t>URI</t>
   </si>
   <si>
@@ -403,9 +400,6 @@
     <t>Bike-hiring Stations</t>
   </si>
   <si>
-    <t>Car-sharing Stations</t>
-  </si>
-  <si>
     <t>E-scooter-sharing Locations and stations</t>
   </si>
   <si>
@@ -475,10 +469,16 @@
     <t>http://purl.org/ontology/bibo/status</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>Published Controlled Vocabulary</t>
+  </si>
+  <si>
+    <t>Car-hiring Stations</t>
+  </si>
+  <si>
+    <t>https://w3id.org/mobilitydcat-ap/mobility-theme/1.0.0</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
   </si>
 </sst>
 </file>
@@ -922,10 +922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +952,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -961,7 +961,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1009,7 +1009,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1019,15 +1019,17 @@
       </c>
       <c r="B10" t="str">
         <f>_xlfn.CONCAT(B1,"/",B9)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/1.0.0</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/1.0.1</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="6"/>
+        <v>132</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1041,81 +1043,85 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="2" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="184.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="str">
+        <f t="shared" ref="A18:A46" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B18,"/","-"))," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/data-content-category</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="184.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="13"/>
+      <c r="D18" s="14" t="str">
+        <f>CONCATENATE(A20,", ",A34,", ",A42,", ",A47,", ",A56,", ",A61,", ",A65,", ",A75,", ",A78,", ",A82,", ",A91,", ",A97,", ",A119,", ",A27,", ",A31,", ",A127,", ",A140,", ",A141,", ",A142)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-road-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/static-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/toll-information, https://w3id.org/mobilitydcat-ap/mobility-theme/parking-service-and-rest-area-information, https://w3id.org/mobilitydcat-ap/mobility-theme/filling-and-charging-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/freight-and-logistics, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/road-work-information, https://w3id.org/mobilitydcat-ap/mobility-theme/road-events-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-traffic-data, https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning-, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-non-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/cycle-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/sharing-and-hiring-services, https://w3id.org/mobilitydcat-ap/mobility-theme/air-and-space-travel, https://w3id.org/mobilitydcat-ap/mobility-theme/waterways-and-water-bodies, https://w3id.org/mobilitydcat-ap/mobility-theme/other</v>
+      </c>
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="1:5" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="str">
-        <f t="shared" ref="A19:A47" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B19,"/","-"))," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/data-content-category</v>
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/data-content-sub-category</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="14" t="str">
-        <f>CONCATENATE(A21,", ",A35,", ",A43,", ",A48,", ",A57,", ",A62,", ",A66,", ",A76,", ",A79,", ",A83,", ",A92,", ",A98,", ",A120,", ",A28,", ",A32,", ",A128,", ",A141,", ",A142,", ",A143)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-road-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/static-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/toll-information, https://w3id.org/mobilitydcat-ap/mobility-theme/parking-service-and-rest-area-information, https://w3id.org/mobilitydcat-ap/mobility-theme/filling-and-charging-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/freight-and-logistics, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/road-work-information, https://w3id.org/mobilitydcat-ap/mobility-theme/road-events-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-traffic-data, https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning-, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-non-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/cycle-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/sharing-and-hiring-services, https://w3id.org/mobilitydcat-ap/mobility-theme/air-and-space-travel, https://w3id.org/mobilitydcat-ap/mobility-theme/waterways-and-water-bodies, https://w3id.org/mobilitydcat-ap/mobility-theme/other</v>
+        <f>CONCATENATE(D20,", ",D34,", ",D42,", ",D47,", ",D56,", ",D61,", ",D65,", ",D75,", ",D78,", ",D82,", ",D91,", ",D97,", ",D119,", ",D27,", ",D31,", ",D127)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/road-width, https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/gradients, https://w3id.org/mobilitydcat-ap/mobility-theme/junctions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans, https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume, https://w3id.org/mobilitydcat-ap/mobility-theme/speed, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays, https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries, https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers, https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places, https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar, https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links, https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators, https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation, https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes, https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information, https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data, https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/fares, https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/data-content-sub-category</v>
-      </c>
-      <c r="B20" s="12" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-road-network-data</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14" t="str">
-        <f>CONCATENATE(D21,", ",D35,", ",D43,", ",D48,", ",D57,", ",D62,", ",D66,", ",D76,", ",D79,", ",D83,", ",D92,", ",D98,", ",D120,", ",D28,", ",D32,", ",D128)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/road-width, https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/gradients, https://w3id.org/mobilitydcat-ap/mobility-theme/junctions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans, https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume, https://w3id.org/mobilitydcat-ap/mobility-theme/speed, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays, https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries, https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers, https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places, https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar, https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links, https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators, https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation, https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes, https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information, https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data, https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/fares, https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
-      </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="str">
+        <f>CONCATENATE(A21,", ",A22,", ",A23,", ",A24,", ",A25,", ",A26)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/road-width, https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/gradients, https://w3id.org/mobilitydcat-ap/mobility-theme/junctions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-road-network-data</v>
-      </c>
-      <c r="B21" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="D21" s="1" t="str">
-        <f>CONCATENATE(A22,", ",A23,", ",A24,", ",A25,", ",A26,", ",A27)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/road-width, https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/gradients, https://w3id.org/mobilitydcat-ap/mobility-theme/junctions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-width</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>22</v>
@@ -1124,7 +1130,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-width</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>23</v>
@@ -1133,7 +1139,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/gradients</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>24</v>
@@ -1142,7 +1148,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/gradients</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/junctions</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>25</v>
@@ -1151,38 +1157,38 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/junctions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification</v>
-      </c>
-      <c r="B27" s="7" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/cycle-network-data</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="str">
+        <f>CONCATENATE(A28,", ",A29,", ",A30)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/cycle-network-data</v>
-      </c>
-      <c r="B28" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="D28" s="1" t="str">
-        <f>CONCATENATE(A29,", ",A30,", ",A31)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>29</v>
@@ -1191,69 +1197,69 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions</v>
-      </c>
-      <c r="B31" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-data</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="str">
+        <f>CONCATENATE(A32,", ",A33)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-data</v>
-      </c>
-      <c r="B32" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>32</v>
-      </c>
-      <c r="D32" s="1" t="str">
-        <f>CONCATENATE(A33,", ",A34)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities</v>
-      </c>
-      <c r="B34" s="15" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-traffic-signs-and-regulations</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="str">
+        <f>CONCATENATE(A35,", ",A36,", ",A37,", ",A38,", ",A39,", ",A40,", ",A41)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-traffic-signs-and-regulations</v>
-      </c>
-      <c r="B35" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="D35" s="1" t="str">
-        <f>CONCATENATE(A36,", ",A37,", ",A38,", ",A39,", ",A40,", ",A41,", ",A42)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>36</v>
@@ -1262,7 +1268,7 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>37</v>
@@ -1271,7 +1277,7 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>38</v>
@@ -1280,7 +1286,7 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>39</v>
@@ -1289,7 +1295,7 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>40</v>
@@ -1298,38 +1304,38 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans</v>
-      </c>
-      <c r="B42" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/toll-information</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="str">
+        <f>CONCATENATE(A43,", ",A44,", ",A45,", ",A46)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/toll-information</v>
-      </c>
-      <c r="B43" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="D43" s="1" t="str">
-        <f>CONCATENATE(A44,", ",A45,", ",A46,", ",A47)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>44</v>
@@ -1338,7 +1344,7 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>45</v>
@@ -1347,74 +1353,74 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls</v>
-      </c>
-      <c r="B47" s="8" t="s">
+        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B47,"/","-"))," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parking-service-and-rest-area-information</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="str">
+        <f>CONCATENATE(A48,", ",A49,", ",A50,", ",A51,", ",A52,", ",A53,", ",A54,", ",A55)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="str">
-        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B48,"/","-"))," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parking-service-and-rest-area-information</v>
-      </c>
-      <c r="B48" s="9" t="s">
+        <f t="shared" ref="A48:A111" si="1">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B48,"/","-"))," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="D48" s="1" t="str">
-        <f>CONCATENATE(A49,", ",A50,", ",A51,", ",A52,", ",A53,", ",A54,", ",A55,", ",A56)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="str">
-        <f t="shared" ref="A49:A112" si="1">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B49,"/","-"))," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions</v>
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>137</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>51</v>
@@ -1423,7 +1429,7 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>52</v>
@@ -1432,38 +1438,38 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations</v>
-      </c>
-      <c r="B56" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/filling-and-charging-stations</v>
+      </c>
+      <c r="B56" s="9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="str">
+        <f>CONCATENATE(A57,", ",A58,", ",A59,", ",A60)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/filling-and-charging-stations</v>
-      </c>
-      <c r="B57" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D57" s="1" t="str">
-        <f>CONCATENATE(A58,", ",A59,", ",A60,", ",A61)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>56</v>
@@ -1472,7 +1478,7 @@
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>57</v>
@@ -1481,38 +1487,38 @@
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations</v>
-      </c>
-      <c r="B61" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-and-logistics</v>
+      </c>
+      <c r="B61" s="9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="str">
+        <f>CONCATENATE(A62,", ",A63,", ",A64)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-and-logistics</v>
-      </c>
-      <c r="B62" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="D62" s="1" t="str">
-        <f>CONCATENATE(A63,", ",A64,", ",A65)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>61</v>
@@ -1521,74 +1527,74 @@
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-traffic-signs-and-regulations</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" s="1" t="str">
+        <f>CONCATENATE(A66,", ",A67,", ",A68,", ",A69,", ",A70,", ",A71,", ",A72,", ",A73,", ",A74)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-traffic-signs-and-regulations</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D66" s="1" t="str">
-        <f>CONCATENATE(A67,", ",A68,", ",A69,", ",A70,", ",A71,", ",A72,", ",A73,", ",A74,", ",A75)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>142</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>64</v>
@@ -1597,7 +1603,7 @@
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>65</v>
@@ -1606,7 +1612,7 @@
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>66</v>
@@ -1615,69 +1621,69 @@
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans</v>
-      </c>
-      <c r="B75" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-work-information</v>
+      </c>
+      <c r="B75" s="9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D75" s="1" t="str">
+        <f>CONCATENATE(A76,", ",A77)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-work-information</v>
-      </c>
-      <c r="B76" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="D76" s="1" t="str">
-        <f>CONCATENATE(A77,", ",A78)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works</v>
-      </c>
-      <c r="B78" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-events-and-conditions</v>
+      </c>
+      <c r="B78" s="9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D78" s="1" t="str">
+        <f>CONCATENATE(A79,", ",A80,", ",A81)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-events-and-conditions</v>
-      </c>
-      <c r="B79" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents</v>
+      </c>
+      <c r="B79" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="D79" s="1" t="str">
-        <f>CONCATENATE(A80,", ",A81,", ",A82)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>73</v>
@@ -1686,38 +1692,38 @@
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions</v>
-      </c>
-      <c r="B82" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-traffic-data</v>
+      </c>
+      <c r="B82" s="9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="str">
+        <f>CONCATENATE(A83,", ",A84,", ",A85,", ",A86,", ",A87,", ",A88,", ",A89,", ",A90)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume, https://w3id.org/mobilitydcat-ap/mobility-theme/speed, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays, https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-traffic-data</v>
-      </c>
-      <c r="B83" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume</v>
+      </c>
+      <c r="B83" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="D83" s="1" t="str">
-        <f>CONCATENATE(A84,", ",A85,", ",A86,", ",A87,", ",A88,", ",A89,", ",A90,", ",A91)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume, https://w3id.org/mobilitydcat-ap/mobility-theme/speed, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays, https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/speed</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>77</v>
@@ -1726,7 +1732,7 @@
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/speed</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>78</v>
@@ -1735,7 +1741,7 @@
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>79</v>
@@ -1744,7 +1750,7 @@
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>80</v>
@@ -1753,7 +1759,7 @@
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>81</v>
@@ -1762,7 +1768,7 @@
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>82</v>
@@ -1771,38 +1777,38 @@
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries</v>
-      </c>
-      <c r="B91" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning-</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="str">
+        <f>CONCATENATE(A92,", ",A93,", ",A94,", ",A95,", ",A96)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers, https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places, https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning-</v>
-      </c>
-      <c r="B92" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="D92" s="1" t="str">
-        <f>CONCATENATE(A93,", ",A94,", ",A95,", ",A96,", ",A97)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers, https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places, https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>86</v>
@@ -1811,7 +1817,7 @@
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>87</v>
@@ -1820,7 +1826,7 @@
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>88</v>
@@ -1829,38 +1835,38 @@
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="312.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs</v>
-      </c>
-      <c r="B97" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-scheduled-transport</v>
+      </c>
+      <c r="B97" s="9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="312.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D97" s="1" t="str">
+        <f>CONCATENATE(A98,", ",A99,", ",A100,", ",A101,", ",A102,", ",A103,", ",A104,", ",A105,", ",A106,", ",A107,", ",A108,", ",A109,", ",A110,", ",A111,", ",A112,", ",A113,", ",A114,", ",A115,", ",A116,", ",A117,", ",A118)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar, https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links, https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators, https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation, https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes, https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-scheduled-transport</v>
-      </c>
-      <c r="B98" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features</v>
+      </c>
+      <c r="B98" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="D98" s="1" t="str">
-        <f>CONCATENATE(A99,", ",A100,", ",A101,", ",A102,", ",A103,", ",A104,", ",A105,", ",A106,", ",A107,", ",A108,", ",A109,", ",A110,", ",A111,", ",A112,", ",A113,", ",A114,", ",A115,", ",A116,", ",A117,", ",A118,", ",A119)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar, https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links, https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators, https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation, https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes, https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>92</v>
@@ -1869,7 +1875,7 @@
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>93</v>
@@ -1878,7 +1884,7 @@
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>94</v>
@@ -1887,7 +1893,7 @@
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>95</v>
@@ -1896,7 +1902,7 @@
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>96</v>
@@ -1905,7 +1911,7 @@
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>97</v>
@@ -1914,7 +1920,7 @@
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>98</v>
@@ -1923,7 +1929,7 @@
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>99</v>
@@ -1932,16 +1938,16 @@
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>133</v>
@@ -1950,16 +1956,16 @@
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>101</v>
@@ -1968,7 +1974,7 @@
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>102</v>
@@ -1976,8 +1982,8 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
+        <f t="shared" ref="A112:A142" si="2">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B112,"/","-"))," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>103</v>
@@ -1985,8 +1991,8 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="str">
-        <f t="shared" ref="A113:A143" si="2">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B113,"/","-"))," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations</v>
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>104</v>
@@ -1995,7 +2001,7 @@
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>105</v>
@@ -2004,7 +2010,7 @@
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>106</v>
@@ -2013,7 +2019,7 @@
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>107</v>
@@ -2022,7 +2028,7 @@
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>108</v>
@@ -2031,38 +2037,38 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A119" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information</v>
-      </c>
-      <c r="B119" s="8" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-non-scheduled-transport</v>
+      </c>
+      <c r="B119" s="9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="D119" s="1" t="str">
+        <f>CONCATENATE(A120,", ",A121,", ",A122,", ",A123,", ",A124,", ",A125,", ",A126)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data, https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/fares, https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-non-scheduled-transport</v>
-      </c>
-      <c r="B120" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="D120" s="1" t="str">
-        <f>CONCATENATE(A121,", ",A122,", ",A123,", ",A124,", ",A125,", ",A126,", ",A127)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data, https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/fares, https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times</v>
       </c>
       <c r="B121" s="8" t="s">
         <v>112</v>
@@ -2071,7 +2077,7 @@
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>113</v>
@@ -2080,7 +2086,7 @@
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/fares</v>
       </c>
       <c r="B123" s="8" t="s">
         <v>114</v>
@@ -2089,7 +2095,7 @@
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/fares</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options</v>
       </c>
       <c r="B124" s="8" t="s">
         <v>115</v>
@@ -2098,7 +2104,7 @@
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles</v>
       </c>
       <c r="B125" s="8" t="s">
         <v>116</v>
@@ -2107,38 +2113,38 @@
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
       <c r="B126" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="197.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/sharing-and-hiring-services</v>
+      </c>
+      <c r="B127" s="9" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
-      </c>
-      <c r="B127" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="197.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D127" s="1" t="str">
+        <f>CONCATENATE(A128,", ",A129,", ",A130,", ",A131,", ",A132,", ",A133,", ",A134,", ",A135,", ",A136,", ",A137,", ",A138,", ",A139)</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/sharing-and-hiring-services</v>
-      </c>
-      <c r="B128" s="9" t="s">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="D128" s="1" t="str">
-        <f>CONCATENATE(A129,", ",A130,", ",A131,", ",A132,", ",A133,", ",A134,", ",A135,", ",A136,", ",A137,", ",A138,", ",A139,", ",A140)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>119</v>
@@ -2147,7 +2153,7 @@
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>120</v>
@@ -2156,118 +2162,109 @@
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-stations</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-stations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
-      </c>
-      <c r="B140" s="8" t="s">
-        <v>103</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/air-and-space-travel</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/air-and-space-travel</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/waterways-and-water-bodies</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/waterways-and-water-bodies</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mobility-theme: v1.1.0, add applicable legislations
</commit_message>
<xml_diff>
--- a/mobility-theme/mobility-theme.xlsx
+++ b/mobility-theme/mobility-theme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabularies\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B15C8CE-EA0E-48B6-B08D-84EED5D6722B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE39B8EF-B4B1-43BB-9A1E-40134310353E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="158">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -100,12 +100,381 @@
     <t>Static road network data</t>
   </si>
   <si>
+    <t>Road width</t>
+  </si>
+  <si>
+    <t>Road classification</t>
+  </si>
+  <si>
+    <t>Cycle network data</t>
+  </si>
+  <si>
+    <t>Pedestrian network data</t>
+  </si>
+  <si>
+    <t>Pedestrian network geometry</t>
+  </si>
+  <si>
+    <t>Pedestrian accessibility facilities</t>
+  </si>
+  <si>
+    <t>Static traffic signs and regulations</t>
+  </si>
+  <si>
+    <t>Tunnel access conditions</t>
+  </si>
+  <si>
+    <t>Bridge access conditions</t>
+  </si>
+  <si>
+    <t>Speed limits</t>
+  </si>
+  <si>
+    <t>Other static traffic signs</t>
+  </si>
+  <si>
+    <t>Permanent access restrictions</t>
+  </si>
+  <si>
+    <t>Other traffic regulations</t>
+  </si>
+  <si>
+    <t>Traffic circulation plans</t>
+  </si>
+  <si>
+    <t>Toll information</t>
+  </si>
+  <si>
+    <t>Location of tolling stations</t>
+  </si>
+  <si>
+    <t>Identification of tolled roads</t>
+  </si>
+  <si>
+    <t>Applicable road user charges and payment methods</t>
+  </si>
+  <si>
+    <t>Payment methods for tolls</t>
+  </si>
+  <si>
+    <t>Parking, service and rest area information</t>
+  </si>
+  <si>
+    <t>Car parking locations and conditions</t>
+  </si>
+  <si>
+    <t>Service and rest area locations and conditions</t>
+  </si>
+  <si>
+    <t>Truck parking locations and conditions</t>
+  </si>
+  <si>
+    <t>Truck parking availability</t>
+  </si>
+  <si>
+    <t>Park and Ride stops</t>
+  </si>
+  <si>
+    <t>Bike-parking locations</t>
+  </si>
+  <si>
+    <t>Filling and charging stations</t>
+  </si>
+  <si>
+    <t>Location and conditions of charging points</t>
+  </si>
+  <si>
+    <t>Location and conditions of filling stations</t>
+  </si>
+  <si>
+    <t>Availability of charging points for electric vehicles</t>
+  </si>
+  <si>
+    <t>Availability of filling stations</t>
+  </si>
+  <si>
+    <t>Freight and logistics</t>
+  </si>
+  <si>
+    <t>Freight delivery regulations</t>
+  </si>
+  <si>
+    <t>Location of delivery areas</t>
+  </si>
+  <si>
+    <t>Availability of delivery areas</t>
+  </si>
+  <si>
+    <t>Other access restrictions and traffic regulations</t>
+  </si>
+  <si>
+    <t>Dynamic overtaking bans on heavy goods vehicles</t>
+  </si>
+  <si>
+    <t>Dynamic speed limits</t>
+  </si>
+  <si>
+    <t>Direction of travel on reversible lanes</t>
+  </si>
+  <si>
+    <t>Other temporary traffic management measures or plans</t>
+  </si>
+  <si>
+    <t>Road work information</t>
+  </si>
+  <si>
+    <t>Long-term road works</t>
+  </si>
+  <si>
+    <t>Short-term road works</t>
+  </si>
+  <si>
+    <t>Road events and conditions</t>
+  </si>
+  <si>
+    <t>Accidents and incidents</t>
+  </si>
+  <si>
+    <t>Poor road conditions</t>
+  </si>
+  <si>
+    <t>Road weather conditions</t>
+  </si>
+  <si>
+    <t>Real-time traffic data</t>
+  </si>
+  <si>
+    <t>Traffic volume</t>
+  </si>
+  <si>
+    <t>Current travel times</t>
+  </si>
+  <si>
+    <t>Predicted travel times</t>
+  </si>
+  <si>
+    <t>Expected delays</t>
+  </si>
+  <si>
+    <t>Waiting time at border crossings to non-EU Member States</t>
+  </si>
+  <si>
+    <t>Traffic data at border crossings to third countries</t>
+  </si>
+  <si>
+    <t>Address identifiers</t>
+  </si>
+  <si>
+    <t>Topographic places</t>
+  </si>
+  <si>
+    <t>Points of interest</t>
+  </si>
+  <si>
+    <t>Parameters needed to calculate environmental factors</t>
+  </si>
+  <si>
+    <t>Parameters needed to calculate costs</t>
+  </si>
+  <si>
+    <t>Public transport scheduled transport</t>
+  </si>
+  <si>
+    <t>Stop facilities location and features</t>
+  </si>
+  <si>
+    <t>Stop facilities geometry and map layout</t>
+  </si>
+  <si>
+    <t>Stop facilities status of features</t>
+  </si>
+  <si>
+    <t>Stop facilities accessibility and paths within facility</t>
+  </si>
+  <si>
+    <t>Connection links</t>
+  </si>
+  <si>
+    <t>Network topology and routes/lines</t>
+  </si>
+  <si>
+    <t>Transport operators</t>
+  </si>
+  <si>
+    <t>Timetables static</t>
+  </si>
+  <si>
+    <t>Hours of operation</t>
+  </si>
+  <si>
+    <t>Vehicle details</t>
+  </si>
+  <si>
+    <t>Environmental standards for vehicles</t>
+  </si>
+  <si>
+    <t>Disruptions, delays, cancellations</t>
+  </si>
+  <si>
+    <t>Basic common standard fares</t>
+  </si>
+  <si>
+    <t>Passenger classes</t>
+  </si>
+  <si>
+    <t>Common fare products</t>
+  </si>
+  <si>
+    <t>Basic commercial conditions</t>
+  </si>
+  <si>
+    <t>Purchase information</t>
+  </si>
+  <si>
+    <t>Public transport non-scheduled transport</t>
+  </si>
+  <si>
+    <t>Service areas and service times</t>
+  </si>
+  <si>
+    <t>Locations and stations</t>
+  </si>
+  <si>
+    <t>Fares</t>
+  </si>
+  <si>
+    <t>Reservation and purchase options</t>
+  </si>
+  <si>
+    <t>Accesibility information for vehicles</t>
+  </si>
+  <si>
+    <t>Sharing and Hiring Services</t>
+  </si>
+  <si>
+    <t>Bike-sharing Locations and stations</t>
+  </si>
+  <si>
+    <t>Car-sharing Locations and stations</t>
+  </si>
+  <si>
+    <t>Bike-hiring Stations</t>
+  </si>
+  <si>
+    <t>E-scooter-sharing Locations and stations</t>
+  </si>
+  <si>
+    <t>Car-sharing Availability</t>
+  </si>
+  <si>
+    <t>Bike sharing Availability</t>
+  </si>
+  <si>
+    <t>Car-hiring Availability</t>
+  </si>
+  <si>
+    <t>Bike-hiring Availability</t>
+  </si>
+  <si>
+    <t>Payment methods</t>
+  </si>
+  <si>
+    <t>Air and space travel</t>
+  </si>
+  <si>
+    <t>Waterways and water bodies</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Real-time estimated departure and arrival times</t>
+  </si>
+  <si>
+    <t>owl:priorVersion</t>
+  </si>
+  <si>
+    <t>Planned interchanges between scheduled services</t>
+  </si>
+  <si>
+    <t>Car parking availability</t>
+  </si>
+  <si>
+    <t>Service and rest area availability</t>
+  </si>
+  <si>
+    <t>Dynamic traffic signs and regulations</t>
+  </si>
+  <si>
+    <t>Road closures and access conditions</t>
+  </si>
+  <si>
+    <t>Lane closures and access conditions</t>
+  </si>
+  <si>
+    <t>Bridge closures and access conditions</t>
+  </si>
+  <si>
+    <t>Tunnel closures and access conditions</t>
+  </si>
+  <si>
+    <t>Mobility Theme</t>
+  </si>
+  <si>
+    <t>Controlled vocabulary for the classification of the theme for a mobility dataset.</t>
+  </si>
+  <si>
+    <t>http://purl.org/ontology/bibo/status</t>
+  </si>
+  <si>
+    <t>Published Controlled Vocabulary</t>
+  </si>
+  <si>
+    <t>Car-hiring Stations</t>
+  </si>
+  <si>
+    <t>General information for trip-planning</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>https://w3id.org/mobilitydcat-ap/mobility-theme/1.0.1</t>
+  </si>
+  <si>
+    <t>Cycle network geometry and lane character</t>
+  </si>
+  <si>
+    <t>dcterms:replacedBy</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/eli/reg_del/2022/670/oj</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/eli/reg_del/2024/490/oj</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/eli/reg_del/2013/885/oj, https://eur-lex.europa.eu/eli/reg_del/2024/490/oj, https://eur-lex.europa.eu/eli/reg_del/2022/670/oj</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/eli/reg_del/2013/885/oj</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/eli/reg_del/2022/670/oj, https://eur-lex.europa.eu/eli/reg/2023/1804/oj</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/eli/reg_del/2022/670/oj, https://eur-lex.europa.eu/eli/reg_del/2013/886/oj</t>
+  </si>
+  <si>
+    <t>owl:deprecated</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/r5r/applicableLegislation^^xsd:anyURI</t>
+  </si>
+  <si>
     <t>Geometry</t>
   </si>
   <si>
-    <t>Road width</t>
-  </si>
-  <si>
     <t>Number of lanes</t>
   </si>
   <si>
@@ -115,12 +484,6 @@
     <t>Junctions</t>
   </si>
   <si>
-    <t>Road classification</t>
-  </si>
-  <si>
-    <t>Cycle network data</t>
-  </si>
-  <si>
     <t>Network geometry and lane character</t>
   </si>
   <si>
@@ -130,355 +493,22 @@
     <t>Network closures/diversions</t>
   </si>
   <si>
-    <t>Pedestrian network data</t>
-  </si>
-  <si>
-    <t>Pedestrian network geometry</t>
-  </si>
-  <si>
-    <t>Pedestrian accessibility facilities</t>
-  </si>
-  <si>
-    <t>Static traffic signs and regulations</t>
-  </si>
-  <si>
-    <t>Tunnel access conditions</t>
-  </si>
-  <si>
-    <t>Bridge access conditions</t>
-  </si>
-  <si>
-    <t>Speed limits</t>
-  </si>
-  <si>
-    <t>Other static traffic signs</t>
-  </si>
-  <si>
-    <t>Permanent access restrictions</t>
-  </si>
-  <si>
-    <t>Other traffic regulations</t>
-  </si>
-  <si>
-    <t>Traffic circulation plans</t>
-  </si>
-  <si>
-    <t>Toll information</t>
-  </si>
-  <si>
-    <t>Location of tolling stations</t>
-  </si>
-  <si>
-    <t>Identification of tolled roads</t>
-  </si>
-  <si>
-    <t>Applicable road user charges and payment methods</t>
-  </si>
-  <si>
-    <t>Payment methods for tolls</t>
-  </si>
-  <si>
-    <t>Parking, service and rest area information</t>
-  </si>
-  <si>
-    <t>Car parking locations and conditions</t>
-  </si>
-  <si>
-    <t>Service and rest area locations and conditions</t>
-  </si>
-  <si>
-    <t>Truck parking locations and conditions</t>
-  </si>
-  <si>
-    <t>Truck parking availability</t>
-  </si>
-  <si>
-    <t>Park and Ride stops</t>
-  </si>
-  <si>
-    <t>Bike-parking locations</t>
-  </si>
-  <si>
-    <t>Filling and charging stations</t>
-  </si>
-  <si>
-    <t>Location and conditions of charging points</t>
-  </si>
-  <si>
-    <t>Location and conditions of filling stations</t>
-  </si>
-  <si>
-    <t>Availability of charging points for electric vehicles</t>
-  </si>
-  <si>
-    <t>Availability of filling stations</t>
-  </si>
-  <si>
-    <t>Freight and logistics</t>
-  </si>
-  <si>
-    <t>Freight delivery regulations</t>
-  </si>
-  <si>
-    <t>Location of delivery areas</t>
-  </si>
-  <si>
-    <t>Availability of delivery areas</t>
-  </si>
-  <si>
-    <t>Other access restrictions and traffic regulations</t>
-  </si>
-  <si>
-    <t>Dynamic overtaking bans on heavy goods vehicles</t>
-  </si>
-  <si>
-    <t>Dynamic speed limits</t>
-  </si>
-  <si>
-    <t>Direction of travel on reversible lanes</t>
-  </si>
-  <si>
-    <t>Other temporary traffic management measures or plans</t>
-  </si>
-  <si>
-    <t>Road work information</t>
-  </si>
-  <si>
-    <t>Long-term road works</t>
-  </si>
-  <si>
-    <t>Short-term road works</t>
-  </si>
-  <si>
-    <t>Road events and conditions</t>
-  </si>
-  <si>
-    <t>Accidents and incidents</t>
-  </si>
-  <si>
-    <t>Poor road conditions</t>
-  </si>
-  <si>
-    <t>Road weather conditions</t>
-  </si>
-  <si>
-    <t>Real-time traffic data</t>
-  </si>
-  <si>
-    <t>Traffic volume</t>
-  </si>
-  <si>
     <t>Speed</t>
   </si>
   <si>
     <t>Location and length of queues</t>
   </si>
   <si>
-    <t>Current travel times</t>
-  </si>
-  <si>
-    <t>Predicted travel times</t>
-  </si>
-  <si>
-    <t>Expected delays</t>
-  </si>
-  <si>
-    <t>Waiting time at border crossings to non-EU Member States</t>
-  </si>
-  <si>
-    <t>Traffic data at border crossings to third countries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General information for trip-planning </t>
-  </si>
-  <si>
-    <t>Address identifiers</t>
-  </si>
-  <si>
-    <t>Topographic places</t>
-  </si>
-  <si>
-    <t>Points of interest</t>
-  </si>
-  <si>
-    <t>Parameters needed to calculate environmental factors</t>
-  </si>
-  <si>
-    <t>Parameters needed to calculate costs</t>
-  </si>
-  <si>
-    <t>Public transport scheduled transport</t>
-  </si>
-  <si>
-    <t>Stop facilities location and features</t>
-  </si>
-  <si>
-    <t>Stop facilities geometry and map layout</t>
-  </si>
-  <si>
-    <t>Stop facilities status of features</t>
-  </si>
-  <si>
-    <t>Stop facilities accessibility and paths within facility</t>
-  </si>
-  <si>
     <t>Operational Calendar</t>
   </si>
   <si>
-    <t>Connection links</t>
-  </si>
-  <si>
-    <t>Network topology and routes/lines</t>
-  </si>
-  <si>
-    <t>Transport operators</t>
-  </si>
-  <si>
-    <t>Timetables static</t>
-  </si>
-  <si>
-    <t>Hours of operation</t>
-  </si>
-  <si>
-    <t>Vehicle details</t>
-  </si>
-  <si>
-    <t>Environmental standards for vehicles</t>
-  </si>
-  <si>
-    <t>Disruptions, delays, cancellations</t>
-  </si>
-  <si>
-    <t>Basic common standard fares</t>
-  </si>
-  <si>
-    <t>Passenger classes</t>
-  </si>
-  <si>
-    <t>Common fare products</t>
-  </si>
-  <si>
     <t>Special Fare Products</t>
   </si>
   <si>
-    <t>Basic commercial conditions</t>
-  </si>
-  <si>
-    <t>Purchase information</t>
-  </si>
-  <si>
-    <t>Public transport non-scheduled transport</t>
-  </si>
-  <si>
     <t>Provider data</t>
   </si>
   <si>
-    <t>Service areas and service times</t>
-  </si>
-  <si>
-    <t>Locations and stations</t>
-  </si>
-  <si>
-    <t>Fares</t>
-  </si>
-  <si>
-    <t>Reservation and purchase options</t>
-  </si>
-  <si>
-    <t>Accesibility information for vehicles</t>
-  </si>
-  <si>
-    <t>Sharing and Hiring Services</t>
-  </si>
-  <si>
-    <t>Bike-sharing Locations and stations</t>
-  </si>
-  <si>
-    <t>Car-sharing Locations and stations</t>
-  </si>
-  <si>
-    <t>Bike-hiring Stations</t>
-  </si>
-  <si>
-    <t>E-scooter-sharing Locations and stations</t>
-  </si>
-  <si>
-    <t>Car-sharing Availability</t>
-  </si>
-  <si>
-    <t>Bike sharing Availability</t>
-  </si>
-  <si>
-    <t>Car-hiring Availability</t>
-  </si>
-  <si>
-    <t>Bike-hiring Availability</t>
-  </si>
-  <si>
     <t>E-scooter-sharing Availability</t>
-  </si>
-  <si>
-    <t>Payment methods</t>
-  </si>
-  <si>
-    <t>Air and space travel</t>
-  </si>
-  <si>
-    <t>Waterways and water bodies</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Real-time estimated departure and arrival times</t>
-  </si>
-  <si>
-    <t>owl:priorVersion</t>
-  </si>
-  <si>
-    <t>Planned interchanges between scheduled services</t>
-  </si>
-  <si>
-    <t>Car parking availability</t>
-  </si>
-  <si>
-    <t>Service and rest area availability</t>
-  </si>
-  <si>
-    <t>Dynamic traffic signs and regulations</t>
-  </si>
-  <si>
-    <t>Road closures and access conditions</t>
-  </si>
-  <si>
-    <t>Lane closures and access conditions</t>
-  </si>
-  <si>
-    <t>Bridge closures and access conditions</t>
-  </si>
-  <si>
-    <t>Tunnel closures and access conditions</t>
-  </si>
-  <si>
-    <t>Mobility Theme</t>
-  </si>
-  <si>
-    <t>Controlled vocabulary for the classification of the theme for a mobility dataset.</t>
-  </si>
-  <si>
-    <t>http://purl.org/ontology/bibo/status</t>
-  </si>
-  <si>
-    <t>Published Controlled Vocabulary</t>
-  </si>
-  <si>
-    <t>Car-hiring Stations</t>
-  </si>
-  <si>
-    <t>https://w3id.org/mobilitydcat-ap/mobility-theme/1.0.0</t>
-  </si>
-  <si>
-    <t>1.0.1</t>
   </si>
 </sst>
 </file>
@@ -914,7 +944,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -922,23 +952,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E142"/>
+  <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="109.140625" customWidth="1"/>
-    <col min="2" max="2" width="87.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="77.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="98.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="8" width="58.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -947,109 +979,98 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="str">
         <f>_xlfn.CONCAT(B1,"/",B9)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/1.0.1</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/1.1.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1065,8 +1086,17 @@
       <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="184.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="str">
         <f t="shared" ref="A18:A46" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B18,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/data-content-category</v>
@@ -1077,11 +1107,12 @@
       <c r="C18" s="13"/>
       <c r="D18" s="14" t="str">
         <f>CONCATENATE(A20,", ",A34,", ",A42,", ",A47,", ",A56,", ",A61,", ",A65,", ",A75,", ",A78,", ",A82,", ",A91,", ",A97,", ",A119,", ",A27,", ",A31,", ",A127,", ",A140,", ",A141,", ",A142)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-road-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/static-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/toll-information, https://w3id.org/mobilitydcat-ap/mobility-theme/parking-service-and-rest-area-information, https://w3id.org/mobilitydcat-ap/mobility-theme/filling-and-charging-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/freight-and-logistics, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/road-work-information, https://w3id.org/mobilitydcat-ap/mobility-theme/road-events-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-traffic-data, https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning-, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-non-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/cycle-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/sharing-and-hiring-services, https://w3id.org/mobilitydcat-ap/mobility-theme/air-and-space-travel, https://w3id.org/mobilitydcat-ap/mobility-theme/waterways-and-water-bodies, https://w3id.org/mobilitydcat-ap/mobility-theme/other</v>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-road-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/static-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/toll-information, https://w3id.org/mobilitydcat-ap/mobility-theme/parking-service-and-rest-area-information, https://w3id.org/mobilitydcat-ap/mobility-theme/filling-and-charging-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/freight-and-logistics, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/road-work-information, https://w3id.org/mobilitydcat-ap/mobility-theme/road-events-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-traffic-data, https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-non-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/cycle-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/sharing-and-hiring-services, https://w3id.org/mobilitydcat-ap/mobility-theme/air-and-space-travel, https://w3id.org/mobilitydcat-ap/mobility-theme/waterways-and-water-bodies, https://w3id.org/mobilitydcat-ap/mobility-theme/other</v>
       </c>
       <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/data-content-sub-category</v>
@@ -1095,8 +1126,9 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/road-width, https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/gradients, https://w3id.org/mobilitydcat-ap/mobility-theme/junctions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans, https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume, https://w3id.org/mobilitydcat-ap/mobility-theme/speed, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays, https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries, https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers, https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places, https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar, https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links, https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators, https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation, https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes, https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information, https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data, https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/fares, https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
       <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-road-network-data</v>
@@ -1108,1163 +1140,1516 @@
         <f>CONCATENATE(A21,", ",A22,", ",A23,", ",A24,", ",A25,", ",A26)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/road-width, https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/gradients, https://w3id.org/mobilitydcat-ap/mobility-theme/junctions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H20" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-width</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/gradients</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/junctions</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/cycle-network-data</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D27" s="1" t="str">
         <f>CONCATENATE(A28,", ",A29,", ",A30)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H27" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-data</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D31" s="1" t="str">
         <f>CONCATENATE(A32,", ",A33)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H31" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-traffic-signs-and-regulations</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D34" s="1" t="str">
         <f>CONCATENATE(A35,", ",A36,", ",A37,", ",A38,", ",A39,", ",A40,", ",A41)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H34" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/toll-information</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D42" s="1" t="str">
         <f>CONCATENATE(A43,", ",A44,", ",A45,", ",A46)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H42" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="str">
         <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B47,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parking-service-and-rest-area-information</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D47" s="1" t="str">
         <f>CONCATENATE(A48,", ",A49,", ",A50,", ",A51,", ",A52,", ",A53,", ",A54,", ",A55)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H47" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="str">
         <f t="shared" ref="A48:A111" si="1">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B48,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/filling-and-charging-stations</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D56" s="1" t="str">
         <f>CONCATENATE(A57,", ",A58,", ",A59,", ",A60)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H56" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-and-logistics</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D61" s="1" t="str">
         <f>CONCATENATE(A62,", ",A63,", ",A64)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H61" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-traffic-signs-and-regulations</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D65" s="1" t="str">
         <f>CONCATENATE(A66,", ",A67,", ",A68,", ",A69,", ",A70,", ",A71,", ",A72,", ",A73,", ",A74)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H65" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-work-information</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D75" s="1" t="str">
         <f>CONCATENATE(A76,", ",A77)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H75" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-events-and-conditions</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D78" s="1" t="str">
         <f>CONCATENATE(A79,", ",A80,", ",A81)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H78" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-traffic-data</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D82" s="1" t="str">
         <f>CONCATENATE(A83,", ",A84,", ",A85,", ",A86,", ",A87,", ",A88,", ",A89,", ",A90)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume, https://w3id.org/mobilitydcat-ap/mobility-theme/speed, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays, https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H82" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/speed</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="H88" s="1"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="H90" s="1"/>
+    </row>
+    <row r="91" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning-</v>
+        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B91,"/","-"))," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
       <c r="D91" s="1" t="str">
         <f>CONCATENATE(A92,", ",A93,", ",A94,", ",A95,", ",A96)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers, https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places, https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H91" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="312.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="H96" s="1"/>
+    </row>
+    <row r="97" spans="1:8" ht="360" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-scheduled-transport</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D97" s="1" t="str">
         <f>CONCATENATE(A98,", ",A99,", ",A100,", ",A101,", ",A102,", ",A103,", ",A104,", ",A105,", ",A106,", ",A107,", ",A108,", ",A109,", ",A110,", ",A111,", ",A112,", ",A113,", ",A114,", ",A115,", ",A116,", ",A117,", ",A118)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar, https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links, https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators, https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation, https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes, https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H97" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features</v>
       </c>
       <c r="B98" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar</v>
-      </c>
-      <c r="B102" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines</v>
-      </c>
-      <c r="B104" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details</v>
-      </c>
-      <c r="B110" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H111" s="1"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="10" t="str">
         <f t="shared" ref="A112:A142" si="2">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B112,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A119" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-non-scheduled-transport</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D119" s="1" t="str">
         <f>CONCATENATE(A120,", ",A121,", ",A122,", ",A123,", ",A124,", ",A125,", ",A126)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data, https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/fares, https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H119" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/fares</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="197.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="H126" s="1"/>
+    </row>
+    <row r="127" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A127" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/sharing-and-hiring-services</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D127" s="1" t="str">
         <f>CONCATENATE(A128,", ",A129,", ",A130,", ",A131,", ",A132,", ",A133,", ",A134,", ",A135,", ",A136,", ",A137,", ",A138,", ",A139)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H127" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-stations</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="H139" s="1"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/air-and-space-travel</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/waterways-and-water-bodies</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="10" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2272,9 +2657,11 @@
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="https://w3id.org/mobilitydcat-ap/data-content-category" xr:uid="{8D37ED2A-6F4C-4B2C-B212-84B5255111B4}"/>
     <hyperlink ref="B12" r:id="rId2" xr:uid="{F5CCEF78-A2AE-420B-8B79-2E74A78B421A}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{048E9DE3-8B8B-4C29-8919-911D84623AFB}"/>
+    <hyperlink ref="H17" r:id="rId4" xr:uid="{F154D901-F5CC-4BA5-8C60-65E6B8A7F74B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2284,35 +2671,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4ea66b1c-fa60-4493-a86c-b420df37761a" xsi:nil="true"/>
-    <Date_x002f_Heure xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <note xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100156B981FAAFB4349A28B03AB4EEECF9F" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1e7c9bb6974a57a0073a8d48fc3b6089">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ea66b1c-fa60-4493-a86c-b420df37761a" xmlns:ns3="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d5753863158ce54f5fdf0d8971fe3971" ns2:_="" ns3:_="">
     <xsd:import namespace="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
@@ -2575,26 +2940,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F704F36C-6F34-42D8-A9E1-097741891E9D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
-    <ds:schemaRef ds:uri="322c47a9-7cf9-4f39-ba36-4bf679c08fb0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4ea66b1c-fa60-4493-a86c-b420df37761a" xsi:nil="true"/>
+    <Date_x002f_Heure xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <note xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{657E47DB-18D8-4B56-B373-635DFCE72B01}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2611,4 +2979,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F704F36C-6F34-42D8-A9E1-097741891E9D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="322c47a9-7cf9-4f39-ba36-4bf679c08fb0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
mobility-theme: v1.1.1 (close #31)
</commit_message>
<xml_diff>
--- a/mobility-theme/mobility-theme.xlsx
+++ b/mobility-theme/mobility-theme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabularies\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE39B8EF-B4B1-43BB-9A1E-40134310353E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F56E28D-EF51-4545-8D0E-13CD000CB86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -436,42 +436,15 @@
     <t>General information for trip-planning</t>
   </si>
   <si>
-    <t>1.1.0</t>
-  </si>
-  <si>
-    <t>https://w3id.org/mobilitydcat-ap/mobility-theme/1.0.1</t>
-  </si>
-  <si>
     <t>Cycle network geometry and lane character</t>
   </si>
   <si>
     <t>dcterms:replacedBy</t>
   </si>
   <si>
-    <t>https://eur-lex.europa.eu/eli/reg_del/2022/670/oj</t>
-  </si>
-  <si>
-    <t>https://eur-lex.europa.eu/eli/reg_del/2024/490/oj</t>
-  </si>
-  <si>
-    <t>https://eur-lex.europa.eu/eli/reg_del/2013/885/oj, https://eur-lex.europa.eu/eli/reg_del/2024/490/oj, https://eur-lex.europa.eu/eli/reg_del/2022/670/oj</t>
-  </si>
-  <si>
-    <t>https://eur-lex.europa.eu/eli/reg_del/2013/885/oj</t>
-  </si>
-  <si>
-    <t>https://eur-lex.europa.eu/eli/reg_del/2022/670/oj, https://eur-lex.europa.eu/eli/reg/2023/1804/oj</t>
-  </si>
-  <si>
-    <t>https://eur-lex.europa.eu/eli/reg_del/2022/670/oj, https://eur-lex.europa.eu/eli/reg_del/2013/886/oj</t>
-  </si>
-  <si>
     <t>owl:deprecated</t>
   </si>
   <si>
-    <t>http://data.europa.eu/r5r/applicableLegislation^^xsd:anyURI</t>
-  </si>
-  <si>
     <t>Geometry</t>
   </si>
   <si>
@@ -509,6 +482,33 @@
   </si>
   <si>
     <t>E-scooter-sharing Availability</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/r5r/applicableLegislation</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/eli/reg_del/2022/670/oj</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/eli/reg_del/2024/490/oj</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/eli/reg_del/2013/885/oj, http://data.europa.eu/eli/reg_del/2024/490/oj, http://data.europa.eu/eli/reg_del/2022/670/oj</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/eli/reg_del/2013/885/oj</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/eli/reg_del/2022/670/oj, http://data.europa.eu/eli/reg/2023/1804/oj</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/eli/reg_del/2022/670/oj, http://data.europa.eu/eli/reg_del/2013/886/oj</t>
+  </si>
+  <si>
+    <t>https://w3id.org/mobilitydcat-ap/mobility-theme/1.1.0</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -635,6 +634,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -944,7 +944,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -954,23 +954,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="98.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="98.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="58.44140625" customWidth="1"/>
+    <col min="8" max="8" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -979,7 +979,7 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -987,7 +987,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -995,7 +995,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1019,50 +1019,50 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="str">
         <f>_xlfn.CONCAT(B1,"/",B9)</f>
-        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/1.1.0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>https://w3id.org/mobilitydcat-ap/mobility-theme/1.1.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>129</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1087,196 +1087,196 @@
         <v>17</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="str">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="390" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="str">
         <f t="shared" ref="A18:A46" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B18,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/data-content-category</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14" t="str">
+      <c r="C18" s="12"/>
+      <c r="D18" s="13" t="str">
         <f>CONCATENATE(A20,", ",A34,", ",A42,", ",A47,", ",A56,", ",A61,", ",A65,", ",A75,", ",A78,", ",A82,", ",A91,", ",A97,", ",A119,", ",A27,", ",A31,", ",A127,", ",A140,", ",A141,", ",A142)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-road-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/static-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/toll-information, https://w3id.org/mobilitydcat-ap/mobility-theme/parking-service-and-rest-area-information, https://w3id.org/mobilitydcat-ap/mobility-theme/filling-and-charging-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/freight-and-logistics, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-traffic-signs-and-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/road-work-information, https://w3id.org/mobilitydcat-ap/mobility-theme/road-events-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-traffic-data, https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-non-scheduled-transport, https://w3id.org/mobilitydcat-ap/mobility-theme/cycle-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-data, https://w3id.org/mobilitydcat-ap/mobility-theme/sharing-and-hiring-services, https://w3id.org/mobilitydcat-ap/mobility-theme/air-and-space-travel, https://w3id.org/mobilitydcat-ap/mobility-theme/waterways-and-water-bodies, https://w3id.org/mobilitydcat-ap/mobility-theme/other</v>
       </c>
-      <c r="E18" s="11"/>
+      <c r="E18" s="10"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="str">
+    <row r="19" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/data-content-sub-category</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14" t="str">
+      <c r="C19" s="12"/>
+      <c r="D19" s="13" t="str">
         <f>CONCATENATE(D20,", ",D34,", ",D42,", ",D47,", ",D56,", ",D61,", ",D65,", ",D75,", ",D78,", ",D82,", ",D91,", ",D97,", ",D119,", ",D27,", ",D31,", ",D127)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/road-width, https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/gradients, https://w3id.org/mobilitydcat-ap/mobility-theme/junctions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans, https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume, https://w3id.org/mobilitydcat-ap/mobility-theme/speed, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays, https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries, https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers, https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places, https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar, https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links, https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators, https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation, https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes, https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information, https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data, https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/fares, https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
-      <c r="E19" s="11"/>
+      <c r="E19" s="10"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="str">
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-road-network-data</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="1" t="str">
         <f>CONCATENATE(A21,", ",A22,", ",A23,", ",A24,", ",A25,", ",A26)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/road-width, https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/gradients, https://w3id.org/mobilitydcat-ap/mobility-theme/junctions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="str">
+      <c r="H20" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/geometry</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>145</v>
+      <c r="B21" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-width</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>21</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/number-of-lanes</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>146</v>
+      <c r="B23" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/gradients</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>147</v>
+      <c r="B24" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/junctions</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>148</v>
+      <c r="B25" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-classification</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/cycle-network-data</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="1" t="str">
         <f>CONCATENATE(A28,", ",A29,", ",A30)</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character, https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes, https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="str">
+      <c r="H27" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-geometry-and-lane-character</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>149</v>
+      <c r="B28" s="7" t="s">
+        <v>140</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-detailed-attributes</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>150</v>
+      <c r="B29" s="7" t="s">
+        <v>141</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-closures-diversions</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>151</v>
+      <c r="B30" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-data</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="1" t="str">
@@ -1284,39 +1284,39 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry, https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-network-geometry</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="14" t="s">
         <v>25</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/pedestrian-accessibility-facilities</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>26</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/static-traffic-signs-and-regulations</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D34" s="1" t="str">
@@ -1324,97 +1324,97 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs, https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-access-conditions</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>28</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-access-conditions</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/speed-limits</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>30</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-static-traffic-signs</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="str">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/permanent-access-restrictions</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>32</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-traffic-regulations</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>33</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-circulation-plans</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/toll-information</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D42" s="1" t="str">
@@ -1422,63 +1422,63 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads, https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-tolling-stations</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/identification-of-tolled-roads</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
         <v>37</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/applicable-road-user-charges-and-payment-methods</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="7" t="s">
         <v>38</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods-for-tolls</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>39</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="144" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="str">
         <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B47,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parking-service-and-rest-area-information</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D47" s="1" t="str">
@@ -1486,109 +1486,109 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="str">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="str">
         <f t="shared" ref="A48:A111" si="1">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B48,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-locations-and-conditions</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-parking-availability</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>120</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-locations-and-conditions</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>42</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-and-rest-area-availability</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>121</v>
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="str">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-locations-and-conditions</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="7" t="s">
         <v>43</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="str">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/truck-parking-availability</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="7" t="s">
         <v>44</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="str">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/park-and-ride-stops</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="7" t="s">
         <v>45</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-parking-locations</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/filling-and-charging-stations</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D56" s="1" t="str">
@@ -1596,63 +1596,63 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="str">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-charging-points</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="7" t="s">
         <v>48</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="str">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-conditions-of-filling-stations</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-charging-points-for-electric-vehicles</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="7" t="s">
         <v>50</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="10" t="str">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-filling-stations</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="7" t="s">
         <v>51</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-and-logistics</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D61" s="1" t="str">
@@ -1660,51 +1660,51 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas, https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/freight-delivery-regulations</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="7" t="s">
         <v>53</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-of-delivery-areas</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="7" t="s">
         <v>54</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/availability-of-delivery-areas</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-traffic-signs-and-regulations</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="8" t="s">
         <v>122</v>
       </c>
       <c r="D65" s="1" t="str">
@@ -1712,123 +1712,123 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits, https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes, https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-closures-and-access-conditions</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="7" t="s">
         <v>123</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/lane-closures-and-access-conditions</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="7" t="s">
         <v>124</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bridge-closures-and-access-conditions</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="7" t="s">
         <v>125</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/tunnel-closures-and-access-conditions</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B69" s="7" t="s">
         <v>126</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-access-restrictions-and-traffic-regulations</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="7" t="s">
         <v>56</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-overtaking-bans-on-heavy-goods-vehicles</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="7" t="s">
         <v>57</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A72" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/dynamic-speed-limits</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="7" t="s">
         <v>58</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/direction-of-travel-on-reversible-lanes</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="7" t="s">
         <v>59</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other-temporary-traffic-management-measures-or-plans</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-work-information</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="8" t="s">
         <v>61</v>
       </c>
       <c r="D75" s="1" t="str">
@@ -1836,39 +1836,39 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works, https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A76" s="10" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/long-term-road-works</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="7" t="s">
         <v>62</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/short-term-road-works</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="7" t="s">
         <v>63</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="10" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-events-and-conditions</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D78" s="1" t="str">
@@ -1876,51 +1876,51 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents, https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="10" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accidents-and-incidents</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="7" t="s">
         <v>65</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A80" s="10" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/poor-road-conditions</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="7" t="s">
         <v>66</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A81" s="10" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/road-weather-conditions</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="7" t="s">
         <v>67</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="10" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-traffic-data</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D82" s="1" t="str">
@@ -1928,107 +1928,107 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume, https://w3id.org/mobilitydcat-ap/mobility-theme/speed, https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues, https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times, https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays, https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states, https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A83" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-volume</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="7" t="s">
         <v>69</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A84" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/speed</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>152</v>
+      <c r="B84" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A85" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/location-and-length-of-queues</v>
       </c>
-      <c r="B85" s="8" t="s">
-        <v>153</v>
+      <c r="B85" s="7" t="s">
+        <v>144</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A86" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/current-travel-times</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" s="7" t="s">
         <v>70</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/predicted-travel-times</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="7" t="s">
         <v>71</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/expected-delays</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" s="7" t="s">
         <v>72</v>
       </c>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A89" s="10" t="str">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/waiting-time-at-border-crossings-to-non-eu-member-states</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" s="7" t="s">
         <v>73</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="10" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/traffic-data-at-border-crossings-to-third-countries</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B90" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A91" s="10" t="str">
+    <row r="91" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="str">
         <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B91,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/general-information-for-trip-planning</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B91" s="8" t="s">
         <v>132</v>
       </c>
       <c r="D91" s="1" t="str">
@@ -2036,73 +2036,73 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers, https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places, https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors, https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/address-identifiers</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" s="7" t="s">
         <v>75</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A93" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/topographic-places</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="B93" s="7" t="s">
         <v>76</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/points-of-interest</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B94" s="7" t="s">
         <v>77</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A95" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-environmental-factors</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="7" t="s">
         <v>78</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/parameters-needed-to-calculate-costs</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B96" s="7" t="s">
         <v>79</v>
       </c>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8" ht="360" x14ac:dyDescent="0.3">
-      <c r="A97" s="10" t="str">
+    <row r="97" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-scheduled-transport</v>
       </c>
-      <c r="B97" s="9" t="s">
+      <c r="B97" s="8" t="s">
         <v>80</v>
       </c>
       <c r="D97" s="1" t="str">
@@ -2110,265 +2110,265 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features, https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility, https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar, https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links, https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines, https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators, https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static, https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times, https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services, https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation, https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares, https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes, https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products, https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions, https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-location-and-features</v>
       </c>
-      <c r="B98" s="8" t="s">
+      <c r="B98" s="7" t="s">
         <v>81</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A99" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-geometry-and-map-layout</v>
       </c>
-      <c r="B99" s="8" t="s">
+      <c r="B99" s="7" t="s">
         <v>82</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-status-of-features</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/stop-facilities-accessibility-and-paths-within-facility</v>
       </c>
-      <c r="B101" s="8" t="s">
+      <c r="B101" s="7" t="s">
         <v>84</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/operational-calendar</v>
       </c>
-      <c r="B102" s="8" t="s">
-        <v>154</v>
+      <c r="B102" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/connection-links</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="B103" s="7" t="s">
         <v>85</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A104" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/network-topology-and-routes-lines</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="7" t="s">
         <v>86</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A105" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/transport-operators</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="B105" s="7" t="s">
         <v>87</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A106" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/timetables-static</v>
       </c>
-      <c r="B106" s="8" t="s">
+      <c r="B106" s="7" t="s">
         <v>88</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A107" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/real-time-estimated-departure-and-arrival-times</v>
       </c>
-      <c r="B107" s="8" t="s">
+      <c r="B107" s="7" t="s">
         <v>117</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A108" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/planned-interchanges-between-scheduled-services</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B108" s="7" t="s">
         <v>119</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A109" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/hours-of-operation</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="B109" s="7" t="s">
         <v>89</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A110" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/vehicle-details</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="B110" s="7" t="s">
         <v>90</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A111" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="str">
         <f t="shared" si="1"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="B111" s="7" t="s">
         <v>91</v>
       </c>
       <c r="H111" s="1"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A112" s="10" t="str">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="9" t="str">
         <f t="shared" ref="A112:A142" si="2">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(B112,"/","-"))," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/disruptions-delays-cancellations</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="B112" s="7" t="s">
         <v>92</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A113" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/basic-common-standard-fares</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="B113" s="7" t="s">
         <v>93</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/passenger-classes</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="B114" s="7" t="s">
         <v>94</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/common-fare-products</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="B115" s="7" t="s">
         <v>95</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/special-fare-products</v>
       </c>
-      <c r="B116" s="8" t="s">
-        <v>155</v>
+      <c r="B116" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/basic-commercial-conditions</v>
       </c>
-      <c r="B117" s="8" t="s">
+      <c r="B117" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A118" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/purchase-information</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="B118" s="7" t="s">
         <v>97</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A119" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A119" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/public-transport-non-scheduled-transport</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B119" s="8" t="s">
         <v>98</v>
       </c>
       <c r="D119" s="1" t="str">
@@ -2376,97 +2376,97 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data, https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times, https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/fares, https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options, https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A120" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/provider-data</v>
       </c>
-      <c r="B120" s="8" t="s">
-        <v>156</v>
+      <c r="B120" s="7" t="s">
+        <v>147</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A121" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/service-areas-and-service-times</v>
       </c>
-      <c r="B121" s="8" t="s">
+      <c r="B121" s="7" t="s">
         <v>99</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A122" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/locations-and-stations</v>
       </c>
-      <c r="B122" s="8" t="s">
+      <c r="B122" s="7" t="s">
         <v>100</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A123" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/fares</v>
       </c>
-      <c r="B123" s="8" t="s">
+      <c r="B123" s="7" t="s">
         <v>101</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A124" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/reservation-and-purchase-options</v>
       </c>
-      <c r="B124" s="8" t="s">
+      <c r="B124" s="7" t="s">
         <v>102</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A125" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/accesibility-information-for-vehicles</v>
       </c>
-      <c r="B125" s="8" t="s">
+      <c r="B125" s="7" t="s">
         <v>103</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A126" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="B126" s="7" t="s">
         <v>91</v>
       </c>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="10" t="str">
+    <row r="127" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+      <c r="A127" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/sharing-and-hiring-services</v>
       </c>
-      <c r="B127" s="9" t="s">
+      <c r="B127" s="8" t="s">
         <v>104</v>
       </c>
       <c r="D127" s="1" t="str">
@@ -2474,181 +2474,181 @@
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations, https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability, https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods, https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-locations-and-stations</v>
       </c>
-      <c r="B128" s="8" t="s">
+      <c r="B128" s="7" t="s">
         <v>105</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A129" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-locations-and-stations</v>
       </c>
-      <c r="B129" s="8" t="s">
+      <c r="B129" s="7" t="s">
         <v>106</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A130" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-stations</v>
       </c>
-      <c r="B130" s="8" t="s">
+      <c r="B130" s="7" t="s">
         <v>107</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A131" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-stations</v>
       </c>
-      <c r="B131" s="8" t="s">
+      <c r="B131" s="7" t="s">
         <v>131</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A132" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-locations-and-stations</v>
       </c>
-      <c r="B132" s="8" t="s">
+      <c r="B132" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A133" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-sharing-availability</v>
       </c>
-      <c r="B133" s="8" t="s">
+      <c r="B133" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-sharing-availability</v>
       </c>
-      <c r="B134" s="8" t="s">
+      <c r="B134" s="7" t="s">
         <v>110</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A135" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/car-hiring-availability</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="B135" s="7" t="s">
         <v>111</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A136" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/bike-hiring-availability</v>
       </c>
-      <c r="B136" s="8" t="s">
+      <c r="B136" s="7" t="s">
         <v>112</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A137" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/e-scooter-sharing-availability</v>
       </c>
-      <c r="B137" s="8" t="s">
-        <v>157</v>
+      <c r="B137" s="7" t="s">
+        <v>148</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A138" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/payment-methods</v>
       </c>
-      <c r="B138" s="8" t="s">
+      <c r="B138" s="7" t="s">
         <v>113</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A139" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/environmental-standards-for-vehicles</v>
       </c>
-      <c r="B139" s="8" t="s">
+      <c r="B139" s="7" t="s">
         <v>91</v>
       </c>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A140" s="10" t="str">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/air-and-space-travel</v>
       </c>
-      <c r="B140" s="9" t="s">
+      <c r="B140" s="8" t="s">
         <v>114</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A141" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/waterways-and-water-bodies</v>
       </c>
-      <c r="B141" s="9" t="s">
+      <c r="B141" s="8" t="s">
         <v>115</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A142" s="10" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="9" t="str">
         <f t="shared" si="2"/>
         <v>https://w3id.org/mobilitydcat-ap/mobility-theme/other</v>
       </c>
-      <c r="B142" s="9" t="s">
+      <c r="B142" s="8" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2656,12 +2656,9 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="https://w3id.org/mobilitydcat-ap/data-content-category" xr:uid="{8D37ED2A-6F4C-4B2C-B212-84B5255111B4}"/>
-    <hyperlink ref="B12" r:id="rId2" xr:uid="{F5CCEF78-A2AE-420B-8B79-2E74A78B421A}"/>
-    <hyperlink ref="B11" r:id="rId3" xr:uid="{048E9DE3-8B8B-4C29-8919-911D84623AFB}"/>
-    <hyperlink ref="H17" r:id="rId4" xr:uid="{F154D901-F5CC-4BA5-8C60-65E6B8A7F74B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2671,13 +2668,35 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4ea66b1c-fa60-4493-a86c-b420df37761a" xsi:nil="true"/>
+    <Date_x002f_Heure xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <note xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100156B981FAAFB4349A28B03AB4EEECF9F" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1e7c9bb6974a57a0073a8d48fc3b6089">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ea66b1c-fa60-4493-a86c-b420df37761a" xmlns:ns3="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d5753863158ce54f5fdf0d8971fe3971" ns2:_="" ns3:_="">
     <xsd:import namespace="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
@@ -2940,29 +2959,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F704F36C-6F34-42D8-A9E1-097741891E9D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="322c47a9-7cf9-4f39-ba36-4bf679c08fb0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4ea66b1c-fa60-4493-a86c-b420df37761a" xsi:nil="true"/>
-    <Date_x002f_Heure xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <note xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{657E47DB-18D8-4B56-B373-635DFCE72B01}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2979,29 +3001,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F704F36C-6F34-42D8-A9E1-097741891E9D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="322c47a9-7cf9-4f39-ba36-4bf679c08fb0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>